<commit_message>
modify Excel and db.json for demo
</commit_message>
<xml_diff>
--- a/src/app/data/example.xlsx
+++ b/src/app/data/example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D_future\front-end\angular-csv\src\app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexwang\Desktop\alexwang_work\angular-csv\src\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62F2AED-B4FB-4D38-91BB-B293E9E20503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F75689-5AA8-4620-97B1-7946A5FDD730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="910" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="910" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="108.06" sheetId="213" state="hidden" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="174">
   <si>
     <t>宗瑋工業股份有限公司Grand Dynasty Industrial Co., Ltd.</t>
   </si>
@@ -1075,22 +1075,26 @@
     <t>PPSU P 3010 本色</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>bar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="m/d;@"/>
-    <numFmt numFmtId="166" formatCode="&quot;T&quot;General"/>
-    <numFmt numFmtId="167" formatCode="&quot;標準：&quot;General\ &quot;T&quot;"/>
-    <numFmt numFmtId="168" formatCode="&quot;成型條件設定事項：各設定值誤差界限 ±&quot;\ General\ &quot;%&quot;"/>
-    <numFmt numFmtId="169" formatCode="&quot;Formation standard setting items: setting tolerance ±&quot;\ General\ &quot;%&quot;"/>
-    <numFmt numFmtId="170" formatCode="#,##0;[Red]#,##0\ &quot;kgs&quot;"/>
-    <numFmt numFmtId="171" formatCode="General\ &quot;kgs&quot;"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="m/d;@"/>
+    <numFmt numFmtId="177" formatCode="&quot;T&quot;General"/>
+    <numFmt numFmtId="178" formatCode="&quot;標準：&quot;General\ &quot;T&quot;"/>
+    <numFmt numFmtId="179" formatCode="&quot;成型條件設定事項：各設定值誤差界限 ±&quot;\ General\ &quot;%&quot;"/>
+    <numFmt numFmtId="180" formatCode="&quot;Formation standard setting items: setting tolerance ±&quot;\ General\ &quot;%&quot;"/>
+    <numFmt numFmtId="181" formatCode="#,##0;[Red]#,##0\ &quot;kgs&quot;"/>
+    <numFmt numFmtId="182" formatCode="General\ &quot;kgs&quot;"/>
   </numFmts>
-  <fonts count="39">
+  <fonts count="40">
     <font>
       <sz val="12"/>
       <name val="新細明體"/>
@@ -1329,7 +1333,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1340,6 +1344,12 @@
       <name val="微軟正黑體"/>
       <family val="2"/>
       <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1589,13 +1599,13 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1608,7 +1618,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="259">
+  <cellXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1651,7 +1661,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="171" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="17" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1660,16 +1670,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
@@ -1807,10 +1817,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1819,13 +1829,13 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="6" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="6" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="6" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1837,13 +1847,13 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="6" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="6" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2041,7 +2051,7 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="13" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2110,16 +2120,16 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="167" fontId="24" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="24" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="23" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="23" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="23" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="23" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="23" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="23" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2386,9 +2396,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="28">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="一般 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="一般 11" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="一般 12" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
@@ -2684,7 +2697,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3011,7 +3024,7 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3027,43 +3040,43 @@
   <dimension ref="A1:AH53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:H16"/>
+      <selection activeCell="S16" sqref="S16:T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.109375" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="5.125" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="5" style="8" customWidth="1"/>
-    <col min="2" max="2" width="1.77734375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="2.6640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="1.75" style="8" customWidth="1"/>
+    <col min="3" max="3" width="2.625" style="8" customWidth="1"/>
     <col min="4" max="4" width="2" style="8" customWidth="1"/>
     <col min="5" max="5" width="3" style="8" customWidth="1"/>
-    <col min="6" max="6" width="0.77734375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="4.33203125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="3.77734375" style="8" customWidth="1"/>
-    <col min="10" max="10" width="3.33203125" style="8" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="0.75" style="8" customWidth="1"/>
+    <col min="7" max="7" width="4.375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="2.625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="3.75" style="8" customWidth="1"/>
+    <col min="10" max="10" width="3.375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="9.125" style="8" customWidth="1"/>
     <col min="12" max="12" width="4" style="8" customWidth="1"/>
-    <col min="13" max="13" width="3.6640625" style="8" customWidth="1"/>
-    <col min="14" max="15" width="6.6640625" style="8" customWidth="1"/>
-    <col min="16" max="16" width="4.109375" style="8" customWidth="1"/>
-    <col min="17" max="17" width="2.33203125" style="8" customWidth="1"/>
-    <col min="18" max="18" width="3.44140625" style="8" customWidth="1"/>
-    <col min="19" max="19" width="5.109375" style="8" customWidth="1"/>
+    <col min="13" max="13" width="3.625" style="8" customWidth="1"/>
+    <col min="14" max="15" width="6.625" style="8" customWidth="1"/>
+    <col min="16" max="16" width="4.125" style="8" customWidth="1"/>
+    <col min="17" max="17" width="2.375" style="8" customWidth="1"/>
+    <col min="18" max="18" width="3.5" style="8" customWidth="1"/>
+    <col min="19" max="19" width="5.125" style="8" customWidth="1"/>
     <col min="20" max="20" width="2" style="8" customWidth="1"/>
-    <col min="21" max="21" width="2.109375" style="8" customWidth="1"/>
-    <col min="22" max="22" width="1.77734375" style="8" customWidth="1"/>
-    <col min="23" max="23" width="3.6640625" style="8" customWidth="1"/>
-    <col min="24" max="24" width="1.88671875" style="8" customWidth="1"/>
-    <col min="25" max="25" width="4.21875" style="8" customWidth="1"/>
-    <col min="26" max="26" width="4.33203125" style="8" customWidth="1"/>
-    <col min="27" max="27" width="4.21875" style="8" customWidth="1"/>
-    <col min="28" max="28" width="3.44140625" style="8" customWidth="1"/>
-    <col min="29" max="31" width="5.109375" style="8" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="10.21875" style="8" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="7.109375" style="8" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="5.109375" style="8" hidden="1" customWidth="1"/>
-    <col min="35" max="16384" width="5.109375" style="8"/>
+    <col min="21" max="21" width="2.125" style="8" customWidth="1"/>
+    <col min="22" max="22" width="1.75" style="8" customWidth="1"/>
+    <col min="23" max="23" width="3.625" style="8" customWidth="1"/>
+    <col min="24" max="24" width="1.875" style="8" customWidth="1"/>
+    <col min="25" max="25" width="4.25" style="8" customWidth="1"/>
+    <col min="26" max="26" width="4.375" style="8" customWidth="1"/>
+    <col min="27" max="27" width="4.25" style="8" customWidth="1"/>
+    <col min="28" max="28" width="3.5" style="8" customWidth="1"/>
+    <col min="29" max="31" width="5.125" style="8" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="10.25" style="8" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="7.125" style="8" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="5.125" style="8" hidden="1" customWidth="1"/>
+    <col min="35" max="16384" width="5.125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="14.25" customHeight="1">
@@ -3737,9 +3750,13 @@
         <v>56</v>
       </c>
       <c r="R14" s="97"/>
-      <c r="S14" s="128"/>
-      <c r="T14" s="128"/>
-      <c r="U14" s="128"/>
+      <c r="S14" s="259">
+        <v>300</v>
+      </c>
+      <c r="T14" s="259"/>
+      <c r="U14" s="128">
+        <v>20</v>
+      </c>
       <c r="V14" s="128"/>
       <c r="W14" s="128"/>
       <c r="X14" s="128"/>
@@ -3781,12 +3798,16 @@
       </c>
       <c r="P15" s="142"/>
       <c r="Q15" s="149" t="s">
-        <v>60</v>
+        <v>173</v>
       </c>
       <c r="R15" s="150"/>
-      <c r="S15" s="128"/>
-      <c r="T15" s="128"/>
-      <c r="U15" s="128"/>
+      <c r="S15" s="259">
+        <v>20</v>
+      </c>
+      <c r="T15" s="259"/>
+      <c r="U15" s="128">
+        <v>20</v>
+      </c>
       <c r="V15" s="128"/>
       <c r="W15" s="128"/>
       <c r="X15" s="128"/>
@@ -3806,7 +3827,7 @@
       </c>
       <c r="AG15" s="24"/>
     </row>
-    <row r="16" spans="1:33" ht="16.2" customHeight="1">
+    <row r="16" spans="1:33" ht="16.149999999999999" customHeight="1">
       <c r="A16" s="133" t="s">
         <v>62</v>
       </c>
@@ -3831,9 +3852,13 @@
         <v>64</v>
       </c>
       <c r="R16" s="132"/>
-      <c r="S16" s="128"/>
-      <c r="T16" s="128"/>
-      <c r="U16" s="128"/>
+      <c r="S16" s="259">
+        <v>80</v>
+      </c>
+      <c r="T16" s="259"/>
+      <c r="U16" s="128">
+        <v>95</v>
+      </c>
       <c r="V16" s="128"/>
       <c r="W16" s="128"/>
       <c r="X16" s="128"/>
@@ -3853,7 +3878,7 @@
       </c>
       <c r="AG16" s="24"/>
     </row>
-    <row r="17" spans="1:32" ht="16.95" customHeight="1">
+    <row r="17" spans="1:32" ht="16.899999999999999" customHeight="1">
       <c r="A17" s="133" t="s">
         <v>66</v>
       </c>
@@ -5311,7 +5336,7 @@
       <c r="AA52" s="66"/>
       <c r="AB52" s="67"/>
     </row>
-    <row r="53" spans="1:28" s="22" customFormat="1" ht="16.95" customHeight="1">
+    <row r="53" spans="1:28" s="22" customFormat="1" ht="16.899999999999999" customHeight="1">
       <c r="A53" s="48" t="s">
         <v>117</v>
       </c>
@@ -5802,12 +5827,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="50.1" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="80.6640625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="20.625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="80.625" style="16" customWidth="1"/>
     <col min="3" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2">
+    <row r="1" spans="1:2" ht="16.5">
       <c r="A1" s="258" t="s">
         <v>122</v>
       </c>
@@ -5844,7 +5869,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="20.25" customHeight="1"/>
-    <row r="7" spans="1:2" ht="16.2">
+    <row r="7" spans="1:2" ht="16.5">
       <c r="A7" s="258" t="s">
         <v>122</v>
       </c>
@@ -5883,7 +5908,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="20.25" customHeight="1"/>
-    <row r="13" spans="1:2" ht="16.2">
+    <row r="13" spans="1:2" ht="16.5">
       <c r="A13" s="258" t="s">
         <v>122</v>
       </c>
@@ -5939,17 +5964,17 @@
       <selection pane="bottomLeft" activeCell="A17" sqref="A17:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="25.2" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="25.15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="40.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="4.21875" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="20.6640625" style="2"/>
+    <col min="1" max="1" width="40.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="4.25" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="20.625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.2" customHeight="1">
+    <row r="1" spans="1:5" ht="25.15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>133</v>
       </c>
@@ -6487,7 +6512,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="25.2" customHeight="1">
+    <row r="33" spans="1:5" ht="25.15" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>168</v>
       </c>
@@ -6504,7 +6529,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="25.2" customHeight="1">
+    <row r="34" spans="1:5" ht="25.15" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>168</v>
       </c>
@@ -6519,7 +6544,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="25.2" customHeight="1">
+    <row r="35" spans="1:5" ht="25.15" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>170</v>
       </c>
@@ -6536,7 +6561,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="25.2" customHeight="1">
+    <row r="36" spans="1:5" ht="25.15" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>172</v>
       </c>
@@ -6551,7 +6576,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="25.2" customHeight="1">
+    <row r="37" spans="1:5" ht="25.15" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>172</v>
       </c>
@@ -6566,7 +6591,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="25.2" customHeight="1">
+    <row r="38" spans="1:5" ht="25.15" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="19"/>
       <c r="C38" s="20" t="s">
@@ -6579,7 +6604,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="25.2" customHeight="1">
+    <row r="39" spans="1:5" ht="25.15" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="19"/>
       <c r="C39" s="20" t="s">
@@ -6592,7 +6617,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="25.2" customHeight="1">
+    <row r="40" spans="1:5" ht="25.15" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="19"/>
       <c r="C40" s="20" t="s">
@@ -6605,7 +6630,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="25.2" customHeight="1">
+    <row r="41" spans="1:5" ht="25.15" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="19"/>
       <c r="C41" s="20" t="s">
@@ -6618,7 +6643,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="25.2" customHeight="1">
+    <row r="42" spans="1:5" ht="25.15" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="19"/>
       <c r="C42" s="20" t="s">
@@ -6631,7 +6656,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="25.2" customHeight="1">
+    <row r="43" spans="1:5" ht="25.15" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="19"/>
       <c r="C43" s="20" t="s">
@@ -6644,7 +6669,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="25.2" customHeight="1">
+    <row r="44" spans="1:5" ht="25.15" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="19"/>
       <c r="C44" s="20" t="s">
@@ -6657,7 +6682,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="25.2" customHeight="1">
+    <row r="45" spans="1:5" ht="25.15" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="19"/>
       <c r="C45" s="20" t="s">
@@ -6670,7 +6695,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="25.2" customHeight="1">
+    <row r="46" spans="1:5" ht="25.15" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="19"/>
       <c r="C46" s="20" t="s">
@@ -6683,7 +6708,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="25.2" customHeight="1">
+    <row r="47" spans="1:5" ht="25.15" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="19"/>
       <c r="C47" s="20" t="s">
@@ -6696,7 +6721,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="25.2" customHeight="1">
+    <row r="48" spans="1:5" ht="25.15" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="19"/>
       <c r="C48" s="20" t="s">
@@ -6709,7 +6734,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="25.2" customHeight="1">
+    <row r="49" spans="1:5" ht="25.15" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="19"/>
       <c r="C49" s="20" t="s">
@@ -6722,7 +6747,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="25.2" customHeight="1">
+    <row r="50" spans="1:5" ht="25.15" customHeight="1">
       <c r="A50" s="1"/>
       <c r="B50" s="19"/>
       <c r="C50" s="20" t="s">
@@ -6735,7 +6760,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="25.2" customHeight="1">
+    <row r="51" spans="1:5" ht="25.15" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="19"/>
       <c r="C51" s="20" t="s">
@@ -6748,7 +6773,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="25.2" customHeight="1">
+    <row r="52" spans="1:5" ht="25.15" customHeight="1">
       <c r="A52" s="1"/>
       <c r="B52" s="19"/>
       <c r="C52" s="20" t="s">
@@ -6761,7 +6786,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="25.2" customHeight="1">
+    <row r="53" spans="1:5" ht="25.15" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="19"/>
       <c r="C53" s="20" t="s">
@@ -6774,7 +6799,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="25.2" customHeight="1">
+    <row r="54" spans="1:5" ht="25.15" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="19"/>
       <c r="C54" s="20" t="s">
@@ -6787,7 +6812,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="25.2" customHeight="1">
+    <row r="55" spans="1:5" ht="25.15" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="19"/>
       <c r="C55" s="20" t="s">
@@ -6800,7 +6825,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="25.2" customHeight="1">
+    <row r="56" spans="1:5" ht="25.15" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="19"/>
       <c r="C56" s="20" t="s">
@@ -6813,7 +6838,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="25.2" customHeight="1">
+    <row r="57" spans="1:5" ht="25.15" customHeight="1">
       <c r="A57" s="1"/>
       <c r="B57" s="19"/>
       <c r="C57" s="20" t="s">
@@ -6826,7 +6851,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="25.2" customHeight="1">
+    <row r="58" spans="1:5" ht="25.15" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="19"/>
       <c r="C58" s="20" t="s">
@@ -6839,7 +6864,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="25.2" customHeight="1">
+    <row r="59" spans="1:5" ht="25.15" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="19"/>
       <c r="C59" s="20" t="s">
@@ -6852,7 +6877,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="25.2" customHeight="1">
+    <row r="60" spans="1:5" ht="25.15" customHeight="1">
       <c r="A60" s="1"/>
       <c r="B60" s="19"/>
       <c r="C60" s="20" t="s">
@@ -6865,7 +6890,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="25.2" customHeight="1">
+    <row r="61" spans="1:5" ht="25.15" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="19"/>
       <c r="C61" s="20" t="s">
@@ -6878,7 +6903,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="25.2" customHeight="1">
+    <row r="62" spans="1:5" ht="25.15" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="19"/>
       <c r="C62" s="20" t="s">
@@ -6891,7 +6916,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="25.2" customHeight="1">
+    <row r="63" spans="1:5" ht="25.15" customHeight="1">
       <c r="A63" s="1"/>
       <c r="B63" s="19"/>
       <c r="C63" s="20" t="s">
@@ -6904,7 +6929,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="25.2" customHeight="1">
+    <row r="64" spans="1:5" ht="25.15" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="19"/>
       <c r="C64" s="20" t="s">
@@ -6917,7 +6942,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="25.2" customHeight="1">
+    <row r="65" spans="1:5" ht="25.15" customHeight="1">
       <c r="A65" s="1"/>
       <c r="B65" s="19"/>
       <c r="C65" s="20" t="s">
@@ -6930,7 +6955,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="25.2" customHeight="1">
+    <row r="66" spans="1:5" ht="25.15" customHeight="1">
       <c r="A66" s="1"/>
       <c r="B66" s="19"/>
       <c r="C66" s="20" t="s">
@@ -6943,7 +6968,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="25.2" customHeight="1">
+    <row r="67" spans="1:5" ht="25.15" customHeight="1">
       <c r="A67" s="1"/>
       <c r="B67" s="19"/>
       <c r="C67" s="20" t="s">
@@ -6956,7 +6981,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="25.2" customHeight="1">
+    <row r="68" spans="1:5" ht="25.15" customHeight="1">
       <c r="A68" s="1"/>
       <c r="B68" s="19"/>
       <c r="C68" s="20" t="s">
@@ -6969,7 +6994,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="25.2" customHeight="1">
+    <row r="69" spans="1:5" ht="25.15" customHeight="1">
       <c r="A69" s="1"/>
       <c r="B69" s="19"/>
       <c r="C69" s="20" t="s">

</xml_diff>

<commit_message>
two sections ejector forms
</commit_message>
<xml_diff>
--- a/src/app/data/example.xlsx
+++ b/src/app/data/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexwang\Desktop\alexwang_work\angular-csv\src\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B86327-50E0-43DE-82F1-EB34BB5867CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC58F5CB-00FC-4BFD-A90F-D32265A1A00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="910" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30765" yWindow="1980" windowWidth="17535" windowHeight="12300" tabRatio="910" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="108.06" sheetId="213" state="hidden" r:id="rId1"/>
@@ -1094,7 +1094,7 @@
     <numFmt numFmtId="181" formatCode="#,##0;[Red]#,##0\ &quot;kgs&quot;"/>
     <numFmt numFmtId="182" formatCode="General\ &quot;kgs&quot;"/>
   </numFmts>
-  <fonts count="39">
+  <fonts count="40">
     <font>
       <sz val="12"/>
       <name val="新細明體"/>
@@ -1345,6 +1345,12 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1612,7 +1618,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="259">
+  <cellXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2070,6 +2076,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="27" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3030,8 +3039,8 @@
   </sheetPr>
   <dimension ref="A1:AH53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AA16" sqref="AA16:AB16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16:W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.125" defaultRowHeight="16.5"/>
@@ -3722,34 +3731,34 @@
       <c r="C14" s="147"/>
       <c r="D14" s="147"/>
       <c r="E14" s="147"/>
-      <c r="F14" s="156"/>
-      <c r="G14" s="156"/>
-      <c r="H14" s="156"/>
+      <c r="F14" s="157"/>
+      <c r="G14" s="157"/>
+      <c r="H14" s="157"/>
       <c r="I14" s="126"/>
       <c r="J14" s="129"/>
       <c r="K14" s="28"/>
       <c r="L14" s="130"/>
       <c r="M14" s="130"/>
-      <c r="N14" s="157" t="s">
+      <c r="N14" s="158" t="s">
         <v>54</v>
       </c>
       <c r="O14" s="123" t="s">
         <v>55</v>
       </c>
-      <c r="P14" s="160"/>
+      <c r="P14" s="161"/>
       <c r="Q14" s="152" t="s">
         <v>56</v>
       </c>
       <c r="R14" s="152"/>
-      <c r="S14" s="130">
-        <v>300</v>
-      </c>
-      <c r="T14" s="130"/>
-      <c r="U14" s="130">
-        <v>20</v>
-      </c>
-      <c r="V14" s="130"/>
-      <c r="W14" s="130"/>
+      <c r="S14" s="153">
+        <v>100</v>
+      </c>
+      <c r="T14" s="153"/>
+      <c r="U14" s="153">
+        <v>400</v>
+      </c>
+      <c r="V14" s="153"/>
+      <c r="W14" s="153"/>
       <c r="X14" s="130"/>
       <c r="Y14" s="130"/>
       <c r="Z14" s="130"/>
@@ -3775,32 +3784,32 @@
       <c r="C15" s="125"/>
       <c r="D15" s="125"/>
       <c r="E15" s="125"/>
-      <c r="F15" s="153"/>
-      <c r="G15" s="153"/>
-      <c r="H15" s="153"/>
+      <c r="F15" s="154"/>
+      <c r="G15" s="154"/>
+      <c r="H15" s="154"/>
       <c r="I15" s="126"/>
       <c r="J15" s="129"/>
       <c r="K15" s="28"/>
       <c r="L15" s="130"/>
       <c r="M15" s="130"/>
-      <c r="N15" s="158"/>
-      <c r="O15" s="154" t="s">
+      <c r="N15" s="159"/>
+      <c r="O15" s="155" t="s">
         <v>59</v>
       </c>
-      <c r="P15" s="155"/>
-      <c r="Q15" s="161" t="s">
+      <c r="P15" s="156"/>
+      <c r="Q15" s="162" t="s">
         <v>173</v>
       </c>
-      <c r="R15" s="162"/>
-      <c r="S15" s="130">
-        <v>20</v>
-      </c>
-      <c r="T15" s="130"/>
-      <c r="U15" s="130">
-        <v>20</v>
-      </c>
-      <c r="V15" s="130"/>
-      <c r="W15" s="130"/>
+      <c r="R15" s="163"/>
+      <c r="S15" s="153">
+        <v>200</v>
+      </c>
+      <c r="T15" s="153"/>
+      <c r="U15" s="153">
+        <v>500</v>
+      </c>
+      <c r="V15" s="153"/>
+      <c r="W15" s="153"/>
       <c r="X15" s="130"/>
       <c r="Y15" s="130"/>
       <c r="Z15" s="130"/>
@@ -3826,32 +3835,32 @@
       <c r="C16" s="125"/>
       <c r="D16" s="125"/>
       <c r="E16" s="125"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
       <c r="I16" s="126"/>
       <c r="J16" s="129"/>
       <c r="K16" s="28"/>
       <c r="L16" s="130"/>
       <c r="M16" s="130"/>
-      <c r="N16" s="158"/>
+      <c r="N16" s="159"/>
       <c r="O16" s="123" t="s">
         <v>63</v>
       </c>
-      <c r="P16" s="171"/>
-      <c r="Q16" s="172" t="s">
+      <c r="P16" s="172"/>
+      <c r="Q16" s="173" t="s">
         <v>64</v>
       </c>
-      <c r="R16" s="173"/>
-      <c r="S16" s="130">
-        <v>80</v>
-      </c>
-      <c r="T16" s="130"/>
-      <c r="U16" s="130">
-        <v>95</v>
-      </c>
-      <c r="V16" s="130"/>
-      <c r="W16" s="130"/>
+      <c r="R16" s="174"/>
+      <c r="S16" s="153">
+        <v>300</v>
+      </c>
+      <c r="T16" s="153"/>
+      <c r="U16" s="153">
+        <v>600</v>
+      </c>
+      <c r="V16" s="153"/>
+      <c r="W16" s="153"/>
       <c r="X16" s="130"/>
       <c r="Y16" s="130"/>
       <c r="Z16" s="130"/>
@@ -3885,15 +3894,15 @@
       <c r="K17" s="28"/>
       <c r="L17" s="130"/>
       <c r="M17" s="130"/>
-      <c r="N17" s="159"/>
+      <c r="N17" s="160"/>
       <c r="O17" s="143" t="s">
         <v>67</v>
       </c>
       <c r="P17" s="151"/>
       <c r="Q17" s="151"/>
       <c r="R17" s="144"/>
-      <c r="S17" s="163"/>
-      <c r="T17" s="163"/>
+      <c r="S17" s="164"/>
+      <c r="T17" s="164"/>
       <c r="U17" s="130"/>
       <c r="V17" s="130"/>
       <c r="W17" s="130"/>
@@ -3924,15 +3933,15 @@
       <c r="F18" s="121"/>
       <c r="G18" s="121"/>
       <c r="H18" s="121"/>
-      <c r="I18" s="169"/>
-      <c r="J18" s="170"/>
+      <c r="I18" s="170"/>
+      <c r="J18" s="171"/>
       <c r="K18" s="7"/>
       <c r="L18" s="121"/>
       <c r="M18" s="121"/>
-      <c r="N18" s="174" t="s">
+      <c r="N18" s="175" t="s">
         <v>70</v>
       </c>
-      <c r="O18" s="164" t="s">
+      <c r="O18" s="165" t="s">
         <v>71</v>
       </c>
       <c r="P18" s="6">
@@ -3974,13 +3983,13 @@
       <c r="F19" s="121"/>
       <c r="G19" s="121"/>
       <c r="H19" s="121"/>
-      <c r="I19" s="169"/>
-      <c r="J19" s="170"/>
+      <c r="I19" s="170"/>
+      <c r="J19" s="171"/>
       <c r="K19" s="7"/>
       <c r="L19" s="121"/>
       <c r="M19" s="121"/>
-      <c r="N19" s="175"/>
-      <c r="O19" s="177"/>
+      <c r="N19" s="176"/>
+      <c r="O19" s="178"/>
       <c r="P19" s="6">
         <v>2</v>
       </c>
@@ -4020,13 +4029,13 @@
       <c r="F20" s="121"/>
       <c r="G20" s="121"/>
       <c r="H20" s="121"/>
-      <c r="I20" s="169"/>
-      <c r="J20" s="170"/>
+      <c r="I20" s="170"/>
+      <c r="J20" s="171"/>
       <c r="K20" s="7"/>
       <c r="L20" s="121"/>
       <c r="M20" s="121"/>
-      <c r="N20" s="175"/>
-      <c r="O20" s="177"/>
+      <c r="N20" s="176"/>
+      <c r="O20" s="178"/>
       <c r="P20" s="6">
         <v>3</v>
       </c>
@@ -4066,13 +4075,13 @@
       <c r="F21" s="121"/>
       <c r="G21" s="121"/>
       <c r="H21" s="121"/>
-      <c r="I21" s="169"/>
-      <c r="J21" s="170"/>
+      <c r="I21" s="170"/>
+      <c r="J21" s="171"/>
       <c r="K21" s="7"/>
       <c r="L21" s="121"/>
       <c r="M21" s="121"/>
-      <c r="N21" s="175"/>
-      <c r="O21" s="177"/>
+      <c r="N21" s="176"/>
+      <c r="O21" s="178"/>
       <c r="P21" s="6">
         <v>4</v>
       </c>
@@ -4096,25 +4105,25 @@
       <c r="AF21" s="24"/>
     </row>
     <row r="22" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A22" s="164" t="s">
+      <c r="A22" s="165" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="166" t="s">
+      <c r="B22" s="167" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="167"/>
-      <c r="D22" s="167"/>
-      <c r="E22" s="168"/>
+      <c r="C22" s="168"/>
+      <c r="D22" s="168"/>
+      <c r="E22" s="169"/>
       <c r="F22" s="121"/>
       <c r="G22" s="121"/>
       <c r="H22" s="121"/>
-      <c r="I22" s="169"/>
-      <c r="J22" s="170"/>
+      <c r="I22" s="170"/>
+      <c r="J22" s="171"/>
       <c r="K22" s="7"/>
       <c r="L22" s="121"/>
       <c r="M22" s="121"/>
-      <c r="N22" s="175"/>
-      <c r="O22" s="177"/>
+      <c r="N22" s="176"/>
+      <c r="O22" s="178"/>
       <c r="P22" s="6">
         <v>5</v>
       </c>
@@ -4144,23 +4153,23 @@
       </c>
     </row>
     <row r="23" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A23" s="165"/>
+      <c r="A23" s="166"/>
       <c r="B23" s="120" t="s">
         <v>81</v>
       </c>
       <c r="C23" s="120"/>
       <c r="D23" s="120"/>
       <c r="E23" s="120"/>
-      <c r="F23" s="169"/>
-      <c r="G23" s="178"/>
-      <c r="H23" s="170"/>
-      <c r="I23" s="169"/>
-      <c r="J23" s="170"/>
+      <c r="F23" s="170"/>
+      <c r="G23" s="179"/>
+      <c r="H23" s="171"/>
+      <c r="I23" s="170"/>
+      <c r="J23" s="171"/>
       <c r="K23" s="7"/>
-      <c r="L23" s="169"/>
-      <c r="M23" s="170"/>
-      <c r="N23" s="175"/>
-      <c r="O23" s="177"/>
+      <c r="L23" s="170"/>
+      <c r="M23" s="171"/>
+      <c r="N23" s="176"/>
+      <c r="O23" s="178"/>
       <c r="P23" s="6">
         <v>6</v>
       </c>
@@ -4168,50 +4177,50 @@
         <v>60</v>
       </c>
       <c r="R23" s="138"/>
-      <c r="S23" s="169"/>
-      <c r="T23" s="170"/>
-      <c r="U23" s="169"/>
-      <c r="V23" s="178"/>
-      <c r="W23" s="170"/>
-      <c r="X23" s="169"/>
-      <c r="Y23" s="178"/>
-      <c r="Z23" s="170"/>
-      <c r="AA23" s="169"/>
-      <c r="AB23" s="170"/>
+      <c r="S23" s="170"/>
+      <c r="T23" s="171"/>
+      <c r="U23" s="170"/>
+      <c r="V23" s="179"/>
+      <c r="W23" s="171"/>
+      <c r="X23" s="170"/>
+      <c r="Y23" s="179"/>
+      <c r="Z23" s="171"/>
+      <c r="AA23" s="170"/>
+      <c r="AB23" s="171"/>
       <c r="AC23" s="24"/>
       <c r="AD23" s="24"/>
       <c r="AE23" s="24"/>
       <c r="AF23" s="24"/>
     </row>
     <row r="24" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A24" s="164" t="s">
+      <c r="A24" s="165" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="166" t="s">
+      <c r="B24" s="167" t="s">
         <v>79</v>
       </c>
-      <c r="C24" s="167"/>
-      <c r="D24" s="167"/>
-      <c r="E24" s="168"/>
+      <c r="C24" s="168"/>
+      <c r="D24" s="168"/>
+      <c r="E24" s="169"/>
       <c r="F24" s="121"/>
       <c r="G24" s="121"/>
       <c r="H24" s="121"/>
-      <c r="I24" s="179"/>
-      <c r="J24" s="180"/>
+      <c r="I24" s="180"/>
+      <c r="J24" s="181"/>
       <c r="K24" s="5"/>
       <c r="L24" s="121"/>
       <c r="M24" s="121"/>
-      <c r="N24" s="175"/>
-      <c r="O24" s="164" t="s">
+      <c r="N24" s="176"/>
+      <c r="O24" s="165" t="s">
         <v>83</v>
       </c>
       <c r="P24" s="6">
         <v>1</v>
       </c>
-      <c r="Q24" s="181" t="s">
+      <c r="Q24" s="182" t="s">
         <v>60</v>
       </c>
-      <c r="R24" s="182"/>
+      <c r="R24" s="183"/>
       <c r="S24" s="121"/>
       <c r="T24" s="121"/>
       <c r="U24" s="121"/>
@@ -4234,7 +4243,7 @@
       </c>
     </row>
     <row r="25" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A25" s="165"/>
+      <c r="A25" s="166"/>
       <c r="B25" s="120" t="s">
         <v>81</v>
       </c>
@@ -4244,13 +4253,13 @@
       <c r="F25" s="121"/>
       <c r="G25" s="121"/>
       <c r="H25" s="121"/>
-      <c r="I25" s="179"/>
-      <c r="J25" s="180"/>
+      <c r="I25" s="180"/>
+      <c r="J25" s="181"/>
       <c r="K25" s="5"/>
       <c r="L25" s="121"/>
       <c r="M25" s="121"/>
-      <c r="N25" s="175"/>
-      <c r="O25" s="177"/>
+      <c r="N25" s="176"/>
+      <c r="O25" s="178"/>
       <c r="P25" s="6">
         <v>2</v>
       </c>
@@ -4290,13 +4299,13 @@
       <c r="F26" s="121"/>
       <c r="G26" s="121"/>
       <c r="H26" s="121"/>
-      <c r="I26" s="179"/>
-      <c r="J26" s="180"/>
+      <c r="I26" s="180"/>
+      <c r="J26" s="181"/>
       <c r="K26" s="5"/>
       <c r="L26" s="121"/>
       <c r="M26" s="121"/>
-      <c r="N26" s="175"/>
-      <c r="O26" s="165"/>
+      <c r="N26" s="176"/>
+      <c r="O26" s="166"/>
       <c r="P26" s="6">
         <v>3</v>
       </c>
@@ -4334,16 +4343,16 @@
       <c r="F27" s="121"/>
       <c r="G27" s="121"/>
       <c r="H27" s="121"/>
-      <c r="I27" s="179"/>
-      <c r="J27" s="180"/>
+      <c r="I27" s="180"/>
+      <c r="J27" s="181"/>
       <c r="K27" s="5"/>
       <c r="L27" s="121"/>
       <c r="M27" s="121"/>
-      <c r="N27" s="175"/>
-      <c r="O27" s="184" t="s">
+      <c r="N27" s="176"/>
+      <c r="O27" s="185" t="s">
         <v>86</v>
       </c>
-      <c r="P27" s="185"/>
+      <c r="P27" s="186"/>
       <c r="Q27" s="138" t="s">
         <v>60</v>
       </c>
@@ -4375,15 +4384,15 @@
         <v>56</v>
       </c>
       <c r="E28" s="152"/>
-      <c r="F28" s="183"/>
-      <c r="G28" s="183"/>
-      <c r="H28" s="183"/>
-      <c r="I28" s="169"/>
-      <c r="J28" s="170"/>
+      <c r="F28" s="184"/>
+      <c r="G28" s="184"/>
+      <c r="H28" s="184"/>
+      <c r="I28" s="170"/>
+      <c r="J28" s="171"/>
       <c r="K28" s="5"/>
       <c r="L28" s="121"/>
       <c r="M28" s="121"/>
-      <c r="N28" s="175"/>
+      <c r="N28" s="176"/>
       <c r="O28" s="120" t="s">
         <v>87</v>
       </c>
@@ -4419,15 +4428,15 @@
         <v>56</v>
       </c>
       <c r="E29" s="152"/>
-      <c r="F29" s="183"/>
-      <c r="G29" s="183"/>
-      <c r="H29" s="183"/>
-      <c r="I29" s="169"/>
-      <c r="J29" s="170"/>
+      <c r="F29" s="184"/>
+      <c r="G29" s="184"/>
+      <c r="H29" s="184"/>
+      <c r="I29" s="170"/>
+      <c r="J29" s="171"/>
       <c r="K29" s="5"/>
       <c r="L29" s="121"/>
       <c r="M29" s="121"/>
-      <c r="N29" s="175"/>
+      <c r="N29" s="176"/>
       <c r="O29" s="120"/>
       <c r="P29" s="6">
         <v>2</v>
@@ -4461,15 +4470,15 @@
         <v>56</v>
       </c>
       <c r="E30" s="152"/>
-      <c r="F30" s="183"/>
-      <c r="G30" s="183"/>
-      <c r="H30" s="183"/>
-      <c r="I30" s="169"/>
-      <c r="J30" s="170"/>
+      <c r="F30" s="184"/>
+      <c r="G30" s="184"/>
+      <c r="H30" s="184"/>
+      <c r="I30" s="170"/>
+      <c r="J30" s="171"/>
       <c r="K30" s="5"/>
       <c r="L30" s="121"/>
       <c r="M30" s="121"/>
-      <c r="N30" s="175"/>
+      <c r="N30" s="176"/>
       <c r="O30" s="120" t="s">
         <v>88</v>
       </c>
@@ -4505,15 +4514,15 @@
         <v>56</v>
       </c>
       <c r="E31" s="152"/>
-      <c r="F31" s="183"/>
-      <c r="G31" s="183"/>
-      <c r="H31" s="183"/>
-      <c r="I31" s="169"/>
-      <c r="J31" s="170"/>
+      <c r="F31" s="184"/>
+      <c r="G31" s="184"/>
+      <c r="H31" s="184"/>
+      <c r="I31" s="170"/>
+      <c r="J31" s="171"/>
       <c r="K31" s="5"/>
       <c r="L31" s="121"/>
       <c r="M31" s="121"/>
-      <c r="N31" s="175"/>
+      <c r="N31" s="176"/>
       <c r="O31" s="120"/>
       <c r="P31" s="6">
         <v>2</v>
@@ -4549,19 +4558,19 @@
         <v>56</v>
       </c>
       <c r="E32" s="152"/>
-      <c r="F32" s="183"/>
-      <c r="G32" s="183"/>
-      <c r="H32" s="183"/>
-      <c r="I32" s="169"/>
-      <c r="J32" s="170"/>
+      <c r="F32" s="184"/>
+      <c r="G32" s="184"/>
+      <c r="H32" s="184"/>
+      <c r="I32" s="170"/>
+      <c r="J32" s="171"/>
       <c r="K32" s="5"/>
       <c r="L32" s="121"/>
       <c r="M32" s="121"/>
-      <c r="N32" s="175"/>
-      <c r="O32" s="186" t="s">
+      <c r="N32" s="176"/>
+      <c r="O32" s="187" t="s">
         <v>91</v>
       </c>
-      <c r="P32" s="187"/>
+      <c r="P32" s="188"/>
       <c r="Q32" s="152" t="s">
         <v>56</v>
       </c>
@@ -4591,19 +4600,19 @@
         <v>56</v>
       </c>
       <c r="E33" s="152"/>
-      <c r="F33" s="183"/>
-      <c r="G33" s="183"/>
-      <c r="H33" s="183"/>
-      <c r="I33" s="169"/>
-      <c r="J33" s="170"/>
+      <c r="F33" s="184"/>
+      <c r="G33" s="184"/>
+      <c r="H33" s="184"/>
+      <c r="I33" s="170"/>
+      <c r="J33" s="171"/>
       <c r="K33" s="5"/>
       <c r="L33" s="121"/>
       <c r="M33" s="121"/>
-      <c r="N33" s="176"/>
-      <c r="O33" s="186" t="s">
+      <c r="N33" s="177"/>
+      <c r="O33" s="187" t="s">
         <v>93</v>
       </c>
-      <c r="P33" s="187"/>
+      <c r="P33" s="188"/>
       <c r="Q33" s="138" t="s">
         <v>60</v>
       </c>
@@ -4620,7 +4629,7 @@
       <c r="AB33" s="121"/>
     </row>
     <row r="34" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A34" s="188" t="s">
+      <c r="A34" s="189" t="s">
         <v>94</v>
       </c>
       <c r="B34" s="120" t="s">
@@ -4631,27 +4640,27 @@
         <v>56</v>
       </c>
       <c r="E34" s="152"/>
-      <c r="F34" s="183"/>
-      <c r="G34" s="183"/>
-      <c r="H34" s="183"/>
-      <c r="I34" s="169"/>
-      <c r="J34" s="170"/>
+      <c r="F34" s="184"/>
+      <c r="G34" s="184"/>
+      <c r="H34" s="184"/>
+      <c r="I34" s="170"/>
+      <c r="J34" s="171"/>
       <c r="K34" s="5"/>
       <c r="L34" s="121"/>
       <c r="M34" s="121"/>
-      <c r="N34" s="174" t="s">
+      <c r="N34" s="175" t="s">
         <v>95</v>
       </c>
-      <c r="O34" s="164" t="s">
+      <c r="O34" s="165" t="s">
         <v>96</v>
       </c>
       <c r="P34" s="6">
         <v>1</v>
       </c>
-      <c r="Q34" s="189" t="s">
+      <c r="Q34" s="190" t="s">
         <v>97</v>
       </c>
-      <c r="R34" s="189"/>
+      <c r="R34" s="190"/>
       <c r="S34" s="121"/>
       <c r="T34" s="121"/>
       <c r="U34" s="121"/>
@@ -4664,7 +4673,7 @@
       <c r="AB34" s="121"/>
     </row>
     <row r="35" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A35" s="188"/>
+      <c r="A35" s="189"/>
       <c r="B35" s="120" t="s">
         <v>92</v>
       </c>
@@ -4673,23 +4682,23 @@
         <v>56</v>
       </c>
       <c r="E35" s="152"/>
-      <c r="F35" s="183"/>
-      <c r="G35" s="183"/>
-      <c r="H35" s="183"/>
-      <c r="I35" s="169"/>
-      <c r="J35" s="170"/>
+      <c r="F35" s="184"/>
+      <c r="G35" s="184"/>
+      <c r="H35" s="184"/>
+      <c r="I35" s="170"/>
+      <c r="J35" s="171"/>
       <c r="K35" s="5"/>
       <c r="L35" s="121"/>
       <c r="M35" s="121"/>
-      <c r="N35" s="175"/>
-      <c r="O35" s="177"/>
+      <c r="N35" s="176"/>
+      <c r="O35" s="178"/>
       <c r="P35" s="6">
         <v>2</v>
       </c>
-      <c r="Q35" s="189" t="s">
+      <c r="Q35" s="190" t="s">
         <v>97</v>
       </c>
-      <c r="R35" s="189"/>
+      <c r="R35" s="190"/>
       <c r="S35" s="121"/>
       <c r="T35" s="121"/>
       <c r="U35" s="121"/>
@@ -4702,34 +4711,34 @@
       <c r="AB35" s="121"/>
     </row>
     <row r="36" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A36" s="164" t="s">
+      <c r="A36" s="165" t="s">
         <v>98</v>
       </c>
       <c r="B36" s="152">
         <v>1</v>
       </c>
       <c r="C36" s="152"/>
-      <c r="D36" s="190" t="s">
+      <c r="D36" s="191" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="190"/>
-      <c r="F36" s="183"/>
-      <c r="G36" s="183"/>
-      <c r="H36" s="183"/>
-      <c r="I36" s="169"/>
-      <c r="J36" s="170"/>
+      <c r="E36" s="191"/>
+      <c r="F36" s="184"/>
+      <c r="G36" s="184"/>
+      <c r="H36" s="184"/>
+      <c r="I36" s="170"/>
+      <c r="J36" s="171"/>
       <c r="K36" s="5"/>
       <c r="L36" s="121"/>
       <c r="M36" s="121"/>
-      <c r="N36" s="175"/>
-      <c r="O36" s="177"/>
+      <c r="N36" s="176"/>
+      <c r="O36" s="178"/>
       <c r="P36" s="6">
         <v>3</v>
       </c>
-      <c r="Q36" s="189" t="s">
+      <c r="Q36" s="190" t="s">
         <v>97</v>
       </c>
-      <c r="R36" s="189"/>
+      <c r="R36" s="190"/>
       <c r="S36" s="121"/>
       <c r="T36" s="121"/>
       <c r="U36" s="121"/>
@@ -4742,32 +4751,32 @@
       <c r="AB36" s="121"/>
     </row>
     <row r="37" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A37" s="177"/>
+      <c r="A37" s="178"/>
       <c r="B37" s="152">
         <v>2</v>
       </c>
       <c r="C37" s="152"/>
-      <c r="D37" s="190" t="s">
+      <c r="D37" s="191" t="s">
         <v>64</v>
       </c>
-      <c r="E37" s="190"/>
-      <c r="F37" s="183"/>
-      <c r="G37" s="183"/>
-      <c r="H37" s="183"/>
-      <c r="I37" s="169"/>
-      <c r="J37" s="170"/>
+      <c r="E37" s="191"/>
+      <c r="F37" s="184"/>
+      <c r="G37" s="184"/>
+      <c r="H37" s="184"/>
+      <c r="I37" s="170"/>
+      <c r="J37" s="171"/>
       <c r="K37" s="5"/>
       <c r="L37" s="121"/>
       <c r="M37" s="121"/>
-      <c r="N37" s="175"/>
-      <c r="O37" s="177"/>
+      <c r="N37" s="176"/>
+      <c r="O37" s="178"/>
       <c r="P37" s="6">
         <v>4</v>
       </c>
-      <c r="Q37" s="189" t="s">
+      <c r="Q37" s="190" t="s">
         <v>97</v>
       </c>
-      <c r="R37" s="189"/>
+      <c r="R37" s="190"/>
       <c r="S37" s="121"/>
       <c r="T37" s="121"/>
       <c r="U37" s="121"/>
@@ -4780,32 +4789,32 @@
       <c r="AB37" s="121"/>
     </row>
     <row r="38" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A38" s="177"/>
+      <c r="A38" s="178"/>
       <c r="B38" s="152">
         <v>3</v>
       </c>
       <c r="C38" s="152"/>
-      <c r="D38" s="190" t="s">
+      <c r="D38" s="191" t="s">
         <v>64</v>
       </c>
-      <c r="E38" s="190"/>
-      <c r="F38" s="183"/>
-      <c r="G38" s="183"/>
-      <c r="H38" s="183"/>
-      <c r="I38" s="169"/>
-      <c r="J38" s="170"/>
+      <c r="E38" s="191"/>
+      <c r="F38" s="184"/>
+      <c r="G38" s="184"/>
+      <c r="H38" s="184"/>
+      <c r="I38" s="170"/>
+      <c r="J38" s="171"/>
       <c r="K38" s="5"/>
       <c r="L38" s="121"/>
       <c r="M38" s="121"/>
-      <c r="N38" s="175"/>
-      <c r="O38" s="177"/>
+      <c r="N38" s="176"/>
+      <c r="O38" s="178"/>
       <c r="P38" s="6">
         <v>5</v>
       </c>
-      <c r="Q38" s="189" t="s">
+      <c r="Q38" s="190" t="s">
         <v>97</v>
       </c>
-      <c r="R38" s="189"/>
+      <c r="R38" s="190"/>
       <c r="S38" s="121"/>
       <c r="T38" s="121"/>
       <c r="U38" s="121"/>
@@ -4818,32 +4827,32 @@
       <c r="AB38" s="121"/>
     </row>
     <row r="39" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A39" s="177"/>
+      <c r="A39" s="178"/>
       <c r="B39" s="152">
         <v>4</v>
       </c>
       <c r="C39" s="152"/>
-      <c r="D39" s="190" t="s">
+      <c r="D39" s="191" t="s">
         <v>64</v>
       </c>
-      <c r="E39" s="190"/>
-      <c r="F39" s="183"/>
-      <c r="G39" s="183"/>
-      <c r="H39" s="183"/>
-      <c r="I39" s="169"/>
-      <c r="J39" s="170"/>
+      <c r="E39" s="191"/>
+      <c r="F39" s="184"/>
+      <c r="G39" s="184"/>
+      <c r="H39" s="184"/>
+      <c r="I39" s="170"/>
+      <c r="J39" s="171"/>
       <c r="K39" s="5"/>
       <c r="L39" s="121"/>
       <c r="M39" s="121"/>
-      <c r="N39" s="175"/>
-      <c r="O39" s="165"/>
+      <c r="N39" s="176"/>
+      <c r="O39" s="166"/>
       <c r="P39" s="6">
         <v>6</v>
       </c>
-      <c r="Q39" s="189" t="s">
+      <c r="Q39" s="190" t="s">
         <v>97</v>
       </c>
-      <c r="R39" s="189"/>
+      <c r="R39" s="190"/>
       <c r="S39" s="121"/>
       <c r="T39" s="121"/>
       <c r="U39" s="121"/>
@@ -4856,34 +4865,34 @@
       <c r="AB39" s="121"/>
     </row>
     <row r="40" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A40" s="177"/>
+      <c r="A40" s="178"/>
       <c r="B40" s="152">
         <v>5</v>
       </c>
       <c r="C40" s="152"/>
-      <c r="D40" s="190" t="s">
+      <c r="D40" s="191" t="s">
         <v>64</v>
       </c>
-      <c r="E40" s="190"/>
-      <c r="F40" s="183"/>
-      <c r="G40" s="183"/>
-      <c r="H40" s="183"/>
-      <c r="I40" s="169"/>
-      <c r="J40" s="170"/>
+      <c r="E40" s="191"/>
+      <c r="F40" s="184"/>
+      <c r="G40" s="184"/>
+      <c r="H40" s="184"/>
+      <c r="I40" s="170"/>
+      <c r="J40" s="171"/>
       <c r="K40" s="5"/>
       <c r="L40" s="121"/>
       <c r="M40" s="121"/>
-      <c r="N40" s="175"/>
+      <c r="N40" s="176"/>
       <c r="O40" s="120" t="s">
         <v>99</v>
       </c>
       <c r="P40" s="6">
         <v>1</v>
       </c>
-      <c r="Q40" s="189" t="s">
+      <c r="Q40" s="190" t="s">
         <v>97</v>
       </c>
-      <c r="R40" s="189"/>
+      <c r="R40" s="190"/>
       <c r="S40" s="121"/>
       <c r="T40" s="121"/>
       <c r="U40" s="121"/>
@@ -4896,32 +4905,32 @@
       <c r="AB40" s="121"/>
     </row>
     <row r="41" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A41" s="177"/>
+      <c r="A41" s="178"/>
       <c r="B41" s="152">
         <v>6</v>
       </c>
       <c r="C41" s="152"/>
-      <c r="D41" s="190" t="s">
+      <c r="D41" s="191" t="s">
         <v>64</v>
       </c>
-      <c r="E41" s="190"/>
-      <c r="F41" s="183"/>
-      <c r="G41" s="183"/>
-      <c r="H41" s="183"/>
-      <c r="I41" s="169"/>
-      <c r="J41" s="170"/>
+      <c r="E41" s="191"/>
+      <c r="F41" s="184"/>
+      <c r="G41" s="184"/>
+      <c r="H41" s="184"/>
+      <c r="I41" s="170"/>
+      <c r="J41" s="171"/>
       <c r="K41" s="5"/>
       <c r="L41" s="121"/>
       <c r="M41" s="121"/>
-      <c r="N41" s="175"/>
+      <c r="N41" s="176"/>
       <c r="O41" s="120"/>
       <c r="P41" s="6">
         <v>2</v>
       </c>
-      <c r="Q41" s="189" t="s">
+      <c r="Q41" s="190" t="s">
         <v>97</v>
       </c>
-      <c r="R41" s="189"/>
+      <c r="R41" s="190"/>
       <c r="S41" s="121"/>
       <c r="T41" s="121"/>
       <c r="U41" s="121"/>
@@ -4934,32 +4943,32 @@
       <c r="AB41" s="121"/>
     </row>
     <row r="42" spans="1:28" ht="18" customHeight="1">
-      <c r="A42" s="186" t="s">
+      <c r="A42" s="187" t="s">
         <v>100</v>
       </c>
-      <c r="B42" s="187"/>
-      <c r="C42" s="187"/>
-      <c r="D42" s="190" t="s">
+      <c r="B42" s="188"/>
+      <c r="C42" s="188"/>
+      <c r="D42" s="191" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="190"/>
-      <c r="F42" s="191"/>
-      <c r="G42" s="191"/>
-      <c r="H42" s="191"/>
-      <c r="I42" s="179"/>
-      <c r="J42" s="180"/>
+      <c r="E42" s="191"/>
+      <c r="F42" s="192"/>
+      <c r="G42" s="192"/>
+      <c r="H42" s="192"/>
+      <c r="I42" s="180"/>
+      <c r="J42" s="181"/>
       <c r="K42" s="5"/>
       <c r="L42" s="121"/>
       <c r="M42" s="121"/>
-      <c r="N42" s="175"/>
+      <c r="N42" s="176"/>
       <c r="O42" s="120"/>
       <c r="P42" s="6">
         <v>3</v>
       </c>
-      <c r="Q42" s="189" t="s">
+      <c r="Q42" s="190" t="s">
         <v>97</v>
       </c>
-      <c r="R42" s="189"/>
+      <c r="R42" s="190"/>
       <c r="S42" s="121"/>
       <c r="T42" s="121"/>
       <c r="U42" s="121"/>
@@ -4972,87 +4981,87 @@
       <c r="AB42" s="121"/>
     </row>
     <row r="43" spans="1:28" ht="20.25" customHeight="1">
-      <c r="A43" s="186" t="s">
+      <c r="A43" s="187" t="s">
         <v>101</v>
       </c>
-      <c r="B43" s="187"/>
-      <c r="C43" s="187"/>
-      <c r="D43" s="192" t="s">
+      <c r="B43" s="188"/>
+      <c r="C43" s="188"/>
+      <c r="D43" s="193" t="s">
         <v>90</v>
       </c>
-      <c r="E43" s="192"/>
+      <c r="E43" s="193"/>
       <c r="F43" s="121"/>
       <c r="G43" s="121"/>
       <c r="H43" s="121"/>
-      <c r="I43" s="179"/>
-      <c r="J43" s="180"/>
+      <c r="I43" s="180"/>
+      <c r="J43" s="181"/>
       <c r="K43" s="5"/>
       <c r="L43" s="121"/>
       <c r="M43" s="121"/>
-      <c r="N43" s="175"/>
-      <c r="O43" s="195" t="s">
+      <c r="N43" s="176"/>
+      <c r="O43" s="196" t="s">
         <v>102</v>
       </c>
-      <c r="P43" s="196"/>
-      <c r="Q43" s="197" t="s">
+      <c r="P43" s="197"/>
+      <c r="Q43" s="198" t="s">
         <v>97</v>
       </c>
-      <c r="R43" s="198"/>
-      <c r="S43" s="199"/>
-      <c r="T43" s="200"/>
-      <c r="U43" s="199"/>
-      <c r="V43" s="201"/>
-      <c r="W43" s="200"/>
-      <c r="X43" s="199"/>
-      <c r="Y43" s="201"/>
-      <c r="Z43" s="200"/>
-      <c r="AA43" s="199"/>
-      <c r="AB43" s="200"/>
+      <c r="R43" s="199"/>
+      <c r="S43" s="200"/>
+      <c r="T43" s="201"/>
+      <c r="U43" s="200"/>
+      <c r="V43" s="202"/>
+      <c r="W43" s="201"/>
+      <c r="X43" s="200"/>
+      <c r="Y43" s="202"/>
+      <c r="Z43" s="201"/>
+      <c r="AA43" s="200"/>
+      <c r="AB43" s="201"/>
     </row>
     <row r="44" spans="1:28" ht="19.5" customHeight="1">
-      <c r="A44" s="186" t="s">
+      <c r="A44" s="187" t="s">
         <v>103</v>
       </c>
-      <c r="B44" s="186"/>
-      <c r="C44" s="186"/>
-      <c r="D44" s="192" t="s">
+      <c r="B44" s="187"/>
+      <c r="C44" s="187"/>
+      <c r="D44" s="193" t="s">
         <v>92</v>
       </c>
-      <c r="E44" s="192"/>
+      <c r="E44" s="193"/>
       <c r="F44" s="121"/>
       <c r="G44" s="121"/>
       <c r="H44" s="121"/>
-      <c r="I44" s="179"/>
-      <c r="J44" s="180"/>
+      <c r="I44" s="180"/>
+      <c r="J44" s="181"/>
       <c r="K44" s="5"/>
       <c r="L44" s="121"/>
       <c r="M44" s="121"/>
-      <c r="N44" s="175"/>
-      <c r="O44" s="193" t="s">
+      <c r="N44" s="176"/>
+      <c r="O44" s="194" t="s">
         <v>104</v>
       </c>
-      <c r="P44" s="194"/>
-      <c r="Q44" s="197" t="s">
+      <c r="P44" s="195"/>
+      <c r="Q44" s="198" t="s">
         <v>97</v>
       </c>
-      <c r="R44" s="198"/>
-      <c r="S44" s="199"/>
-      <c r="T44" s="200"/>
-      <c r="U44" s="203"/>
-      <c r="V44" s="204"/>
-      <c r="W44" s="205"/>
-      <c r="X44" s="199"/>
-      <c r="Y44" s="201"/>
-      <c r="Z44" s="200"/>
-      <c r="AA44" s="199"/>
-      <c r="AB44" s="200"/>
+      <c r="R44" s="199"/>
+      <c r="S44" s="200"/>
+      <c r="T44" s="201"/>
+      <c r="U44" s="204"/>
+      <c r="V44" s="205"/>
+      <c r="W44" s="206"/>
+      <c r="X44" s="200"/>
+      <c r="Y44" s="202"/>
+      <c r="Z44" s="201"/>
+      <c r="AA44" s="200"/>
+      <c r="AB44" s="201"/>
     </row>
     <row r="45" spans="1:28" ht="19.5" customHeight="1">
-      <c r="A45" s="186" t="s">
+      <c r="A45" s="187" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="186"/>
-      <c r="C45" s="186"/>
+      <c r="B45" s="187"/>
+      <c r="C45" s="187"/>
       <c r="D45" s="152" t="s">
         <v>60</v>
       </c>
@@ -5060,25 +5069,25 @@
       <c r="F45" s="121"/>
       <c r="G45" s="121"/>
       <c r="H45" s="121"/>
-      <c r="I45" s="179"/>
-      <c r="J45" s="180"/>
+      <c r="I45" s="180"/>
+      <c r="J45" s="181"/>
       <c r="K45" s="5"/>
       <c r="L45" s="121"/>
       <c r="M45" s="121"/>
-      <c r="N45" s="175"/>
-      <c r="O45" s="223" t="s">
+      <c r="N45" s="176"/>
+      <c r="O45" s="224" t="s">
         <v>106</v>
       </c>
-      <c r="P45" s="224"/>
-      <c r="Q45" s="189" t="s">
+      <c r="P45" s="225"/>
+      <c r="Q45" s="190" t="s">
         <v>97</v>
       </c>
-      <c r="R45" s="189"/>
+      <c r="R45" s="190"/>
       <c r="S45" s="121"/>
       <c r="T45" s="121"/>
-      <c r="U45" s="202"/>
-      <c r="V45" s="202"/>
-      <c r="W45" s="202"/>
+      <c r="U45" s="203"/>
+      <c r="V45" s="203"/>
+      <c r="W45" s="203"/>
       <c r="X45" s="121"/>
       <c r="Y45" s="121"/>
       <c r="Z45" s="121"/>
@@ -5089,34 +5098,34 @@
       <c r="A46" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="B46" s="232"/>
+      <c r="B46" s="233"/>
       <c r="C46" s="94"/>
-      <c r="D46" s="211" t="s">
+      <c r="D46" s="212" t="s">
         <v>108</v>
       </c>
-      <c r="E46" s="212"/>
-      <c r="F46" s="199"/>
-      <c r="G46" s="201"/>
-      <c r="H46" s="200"/>
-      <c r="I46" s="218"/>
-      <c r="J46" s="219"/>
-      <c r="K46" s="209"/>
-      <c r="L46" s="199"/>
-      <c r="M46" s="200"/>
-      <c r="N46" s="175"/>
-      <c r="O46" s="223" t="s">
+      <c r="E46" s="213"/>
+      <c r="F46" s="200"/>
+      <c r="G46" s="202"/>
+      <c r="H46" s="201"/>
+      <c r="I46" s="219"/>
+      <c r="J46" s="220"/>
+      <c r="K46" s="210"/>
+      <c r="L46" s="200"/>
+      <c r="M46" s="201"/>
+      <c r="N46" s="176"/>
+      <c r="O46" s="224" t="s">
         <v>109</v>
       </c>
-      <c r="P46" s="224"/>
-      <c r="Q46" s="189" t="s">
+      <c r="P46" s="225"/>
+      <c r="Q46" s="190" t="s">
         <v>97</v>
       </c>
-      <c r="R46" s="189"/>
+      <c r="R46" s="190"/>
       <c r="S46" s="121"/>
       <c r="T46" s="121"/>
-      <c r="U46" s="202"/>
-      <c r="V46" s="202"/>
-      <c r="W46" s="202"/>
+      <c r="U46" s="203"/>
+      <c r="V46" s="203"/>
+      <c r="W46" s="203"/>
       <c r="X46" s="121"/>
       <c r="Y46" s="121"/>
       <c r="Z46" s="121"/>
@@ -5125,229 +5134,229 @@
     </row>
     <row r="47" spans="1:28" ht="21.75" customHeight="1">
       <c r="A47" s="95"/>
-      <c r="B47" s="233"/>
+      <c r="B47" s="234"/>
       <c r="C47" s="96"/>
-      <c r="D47" s="213"/>
-      <c r="E47" s="214"/>
-      <c r="F47" s="215"/>
-      <c r="G47" s="216"/>
-      <c r="H47" s="217"/>
-      <c r="I47" s="220"/>
-      <c r="J47" s="221"/>
-      <c r="K47" s="222"/>
-      <c r="L47" s="215"/>
-      <c r="M47" s="217"/>
-      <c r="N47" s="175"/>
-      <c r="O47" s="206" t="s">
+      <c r="D47" s="214"/>
+      <c r="E47" s="215"/>
+      <c r="F47" s="216"/>
+      <c r="G47" s="217"/>
+      <c r="H47" s="218"/>
+      <c r="I47" s="221"/>
+      <c r="J47" s="222"/>
+      <c r="K47" s="223"/>
+      <c r="L47" s="216"/>
+      <c r="M47" s="218"/>
+      <c r="N47" s="176"/>
+      <c r="O47" s="207" t="s">
         <v>110</v>
       </c>
-      <c r="P47" s="207"/>
-      <c r="Q47" s="208" t="s">
+      <c r="P47" s="208"/>
+      <c r="Q47" s="209" t="s">
         <v>97</v>
       </c>
-      <c r="R47" s="208"/>
-      <c r="S47" s="209"/>
-      <c r="T47" s="209"/>
-      <c r="U47" s="210"/>
-      <c r="V47" s="210"/>
-      <c r="W47" s="210"/>
-      <c r="X47" s="209"/>
-      <c r="Y47" s="209"/>
-      <c r="Z47" s="209"/>
-      <c r="AA47" s="209"/>
-      <c r="AB47" s="209"/>
+      <c r="R47" s="209"/>
+      <c r="S47" s="210"/>
+      <c r="T47" s="210"/>
+      <c r="U47" s="211"/>
+      <c r="V47" s="211"/>
+      <c r="W47" s="211"/>
+      <c r="X47" s="210"/>
+      <c r="Y47" s="210"/>
+      <c r="Z47" s="210"/>
+      <c r="AA47" s="210"/>
+      <c r="AB47" s="210"/>
     </row>
     <row r="48" spans="1:28" s="9" customFormat="1" ht="12" customHeight="1">
-      <c r="A48" s="243">
+      <c r="A48" s="244">
         <v>10</v>
       </c>
-      <c r="B48" s="244"/>
-      <c r="C48" s="244"/>
-      <c r="D48" s="244"/>
-      <c r="E48" s="244"/>
-      <c r="F48" s="244"/>
-      <c r="G48" s="244"/>
-      <c r="H48" s="244"/>
-      <c r="I48" s="244"/>
-      <c r="J48" s="244"/>
-      <c r="K48" s="244"/>
-      <c r="L48" s="244"/>
-      <c r="M48" s="245"/>
-      <c r="N48" s="246" t="s">
+      <c r="B48" s="245"/>
+      <c r="C48" s="245"/>
+      <c r="D48" s="245"/>
+      <c r="E48" s="245"/>
+      <c r="F48" s="245"/>
+      <c r="G48" s="245"/>
+      <c r="H48" s="245"/>
+      <c r="I48" s="245"/>
+      <c r="J48" s="245"/>
+      <c r="K48" s="245"/>
+      <c r="L48" s="245"/>
+      <c r="M48" s="246"/>
+      <c r="N48" s="247" t="s">
         <v>111</v>
       </c>
-      <c r="O48" s="247"/>
-      <c r="P48" s="247"/>
-      <c r="Q48" s="247"/>
-      <c r="R48" s="247"/>
-      <c r="S48" s="247"/>
-      <c r="T48" s="247"/>
-      <c r="U48" s="247"/>
-      <c r="V48" s="247"/>
-      <c r="W48" s="247"/>
-      <c r="X48" s="247"/>
-      <c r="Y48" s="247"/>
-      <c r="Z48" s="247"/>
-      <c r="AA48" s="247"/>
-      <c r="AB48" s="248"/>
+      <c r="O48" s="248"/>
+      <c r="P48" s="248"/>
+      <c r="Q48" s="248"/>
+      <c r="R48" s="248"/>
+      <c r="S48" s="248"/>
+      <c r="T48" s="248"/>
+      <c r="U48" s="248"/>
+      <c r="V48" s="248"/>
+      <c r="W48" s="248"/>
+      <c r="X48" s="248"/>
+      <c r="Y48" s="248"/>
+      <c r="Z48" s="248"/>
+      <c r="AA48" s="248"/>
+      <c r="AB48" s="249"/>
     </row>
     <row r="49" spans="1:28" s="9" customFormat="1" ht="12" customHeight="1">
-      <c r="A49" s="249">
+      <c r="A49" s="250">
         <v>10</v>
       </c>
-      <c r="B49" s="250"/>
-      <c r="C49" s="250"/>
-      <c r="D49" s="250"/>
-      <c r="E49" s="250"/>
-      <c r="F49" s="250"/>
-      <c r="G49" s="250"/>
-      <c r="H49" s="250"/>
-      <c r="I49" s="250"/>
-      <c r="J49" s="250"/>
-      <c r="K49" s="250"/>
-      <c r="L49" s="250"/>
-      <c r="M49" s="251"/>
-      <c r="N49" s="252" t="s">
+      <c r="B49" s="251"/>
+      <c r="C49" s="251"/>
+      <c r="D49" s="251"/>
+      <c r="E49" s="251"/>
+      <c r="F49" s="251"/>
+      <c r="G49" s="251"/>
+      <c r="H49" s="251"/>
+      <c r="I49" s="251"/>
+      <c r="J49" s="251"/>
+      <c r="K49" s="251"/>
+      <c r="L49" s="251"/>
+      <c r="M49" s="252"/>
+      <c r="N49" s="253" t="s">
         <v>112</v>
       </c>
-      <c r="O49" s="253"/>
-      <c r="P49" s="253"/>
-      <c r="Q49" s="253"/>
-      <c r="R49" s="253"/>
-      <c r="S49" s="253"/>
-      <c r="T49" s="253"/>
-      <c r="U49" s="253"/>
-      <c r="V49" s="253"/>
-      <c r="W49" s="253"/>
-      <c r="X49" s="253"/>
-      <c r="Y49" s="253"/>
-      <c r="Z49" s="253"/>
-      <c r="AA49" s="253"/>
-      <c r="AB49" s="254"/>
+      <c r="O49" s="254"/>
+      <c r="P49" s="254"/>
+      <c r="Q49" s="254"/>
+      <c r="R49" s="254"/>
+      <c r="S49" s="254"/>
+      <c r="T49" s="254"/>
+      <c r="U49" s="254"/>
+      <c r="V49" s="254"/>
+      <c r="W49" s="254"/>
+      <c r="X49" s="254"/>
+      <c r="Y49" s="254"/>
+      <c r="Z49" s="254"/>
+      <c r="AA49" s="254"/>
+      <c r="AB49" s="255"/>
     </row>
     <row r="50" spans="1:28" s="9" customFormat="1" ht="12" customHeight="1">
-      <c r="A50" s="255" t="s">
+      <c r="A50" s="256" t="s">
         <v>113</v>
       </c>
-      <c r="B50" s="256"/>
-      <c r="C50" s="256"/>
-      <c r="D50" s="256"/>
-      <c r="E50" s="256"/>
-      <c r="F50" s="256"/>
-      <c r="G50" s="256"/>
-      <c r="H50" s="256"/>
-      <c r="I50" s="256"/>
-      <c r="J50" s="256"/>
-      <c r="K50" s="256"/>
-      <c r="L50" s="256"/>
-      <c r="M50" s="257"/>
-      <c r="N50" s="234" t="s">
+      <c r="B50" s="257"/>
+      <c r="C50" s="257"/>
+      <c r="D50" s="257"/>
+      <c r="E50" s="257"/>
+      <c r="F50" s="257"/>
+      <c r="G50" s="257"/>
+      <c r="H50" s="257"/>
+      <c r="I50" s="257"/>
+      <c r="J50" s="257"/>
+      <c r="K50" s="257"/>
+      <c r="L50" s="257"/>
+      <c r="M50" s="258"/>
+      <c r="N50" s="235" t="s">
         <v>114</v>
       </c>
-      <c r="O50" s="235"/>
-      <c r="P50" s="235"/>
-      <c r="Q50" s="235"/>
-      <c r="R50" s="235"/>
-      <c r="S50" s="235"/>
-      <c r="T50" s="235"/>
-      <c r="U50" s="235"/>
-      <c r="V50" s="235"/>
-      <c r="W50" s="235"/>
-      <c r="X50" s="235"/>
-      <c r="Y50" s="235"/>
-      <c r="Z50" s="235"/>
-      <c r="AA50" s="235"/>
-      <c r="AB50" s="236"/>
+      <c r="O50" s="236"/>
+      <c r="P50" s="236"/>
+      <c r="Q50" s="236"/>
+      <c r="R50" s="236"/>
+      <c r="S50" s="236"/>
+      <c r="T50" s="236"/>
+      <c r="U50" s="236"/>
+      <c r="V50" s="236"/>
+      <c r="W50" s="236"/>
+      <c r="X50" s="236"/>
+      <c r="Y50" s="236"/>
+      <c r="Z50" s="236"/>
+      <c r="AA50" s="236"/>
+      <c r="AB50" s="237"/>
     </row>
     <row r="51" spans="1:28" s="9" customFormat="1" ht="12" customHeight="1">
-      <c r="A51" s="229" t="s">
+      <c r="A51" s="230" t="s">
         <v>115</v>
       </c>
-      <c r="B51" s="230"/>
-      <c r="C51" s="230"/>
-      <c r="D51" s="230"/>
-      <c r="E51" s="230"/>
-      <c r="F51" s="230"/>
-      <c r="G51" s="230"/>
-      <c r="H51" s="230"/>
-      <c r="I51" s="230"/>
-      <c r="J51" s="230"/>
-      <c r="K51" s="230"/>
-      <c r="L51" s="230"/>
-      <c r="M51" s="231"/>
-      <c r="N51" s="234"/>
-      <c r="O51" s="235"/>
-      <c r="P51" s="235"/>
-      <c r="Q51" s="235"/>
-      <c r="R51" s="235"/>
-      <c r="S51" s="235"/>
-      <c r="T51" s="235"/>
-      <c r="U51" s="235"/>
-      <c r="V51" s="235"/>
-      <c r="W51" s="235"/>
-      <c r="X51" s="235"/>
-      <c r="Y51" s="235"/>
-      <c r="Z51" s="235"/>
-      <c r="AA51" s="235"/>
-      <c r="AB51" s="236"/>
+      <c r="B51" s="231"/>
+      <c r="C51" s="231"/>
+      <c r="D51" s="231"/>
+      <c r="E51" s="231"/>
+      <c r="F51" s="231"/>
+      <c r="G51" s="231"/>
+      <c r="H51" s="231"/>
+      <c r="I51" s="231"/>
+      <c r="J51" s="231"/>
+      <c r="K51" s="231"/>
+      <c r="L51" s="231"/>
+      <c r="M51" s="232"/>
+      <c r="N51" s="235"/>
+      <c r="O51" s="236"/>
+      <c r="P51" s="236"/>
+      <c r="Q51" s="236"/>
+      <c r="R51" s="236"/>
+      <c r="S51" s="236"/>
+      <c r="T51" s="236"/>
+      <c r="U51" s="236"/>
+      <c r="V51" s="236"/>
+      <c r="W51" s="236"/>
+      <c r="X51" s="236"/>
+      <c r="Y51" s="236"/>
+      <c r="Z51" s="236"/>
+      <c r="AA51" s="236"/>
+      <c r="AB51" s="237"/>
     </row>
     <row r="52" spans="1:28" s="9" customFormat="1" ht="12" customHeight="1">
-      <c r="A52" s="226" t="s">
+      <c r="A52" s="227" t="s">
         <v>116</v>
       </c>
-      <c r="B52" s="227"/>
-      <c r="C52" s="227"/>
-      <c r="D52" s="227"/>
-      <c r="E52" s="227"/>
-      <c r="F52" s="227"/>
-      <c r="G52" s="227"/>
-      <c r="H52" s="227"/>
-      <c r="I52" s="227"/>
-      <c r="J52" s="227"/>
-      <c r="K52" s="227"/>
-      <c r="L52" s="227"/>
-      <c r="M52" s="228"/>
-      <c r="N52" s="237" t="s">
+      <c r="B52" s="228"/>
+      <c r="C52" s="228"/>
+      <c r="D52" s="228"/>
+      <c r="E52" s="228"/>
+      <c r="F52" s="228"/>
+      <c r="G52" s="228"/>
+      <c r="H52" s="228"/>
+      <c r="I52" s="228"/>
+      <c r="J52" s="228"/>
+      <c r="K52" s="228"/>
+      <c r="L52" s="228"/>
+      <c r="M52" s="229"/>
+      <c r="N52" s="238" t="s">
         <v>13</v>
       </c>
-      <c r="O52" s="238"/>
-      <c r="P52" s="238"/>
-      <c r="Q52" s="238"/>
-      <c r="R52" s="238"/>
-      <c r="S52" s="238"/>
-      <c r="T52" s="238"/>
-      <c r="U52" s="238"/>
-      <c r="V52" s="238"/>
-      <c r="W52" s="238"/>
-      <c r="X52" s="238"/>
-      <c r="Y52" s="238"/>
-      <c r="Z52" s="239" t="s">
+      <c r="O52" s="239"/>
+      <c r="P52" s="239"/>
+      <c r="Q52" s="239"/>
+      <c r="R52" s="239"/>
+      <c r="S52" s="239"/>
+      <c r="T52" s="239"/>
+      <c r="U52" s="239"/>
+      <c r="V52" s="239"/>
+      <c r="W52" s="239"/>
+      <c r="X52" s="239"/>
+      <c r="Y52" s="239"/>
+      <c r="Z52" s="240" t="s">
         <v>13</v>
       </c>
-      <c r="AA52" s="239"/>
-      <c r="AB52" s="240"/>
+      <c r="AA52" s="240"/>
+      <c r="AB52" s="241"/>
     </row>
     <row r="53" spans="1:28" s="22" customFormat="1" ht="16.899999999999999" customHeight="1">
-      <c r="A53" s="225" t="s">
+      <c r="A53" s="226" t="s">
         <v>117</v>
       </c>
-      <c r="B53" s="225"/>
-      <c r="C53" s="225"/>
-      <c r="D53" s="225"/>
-      <c r="E53" s="225"/>
+      <c r="B53" s="226"/>
+      <c r="C53" s="226"/>
+      <c r="D53" s="226"/>
+      <c r="E53" s="226"/>
       <c r="F53" s="21"/>
-      <c r="G53" s="225" t="s">
+      <c r="G53" s="226" t="s">
         <v>118</v>
       </c>
-      <c r="H53" s="225"/>
-      <c r="I53" s="225"/>
-      <c r="J53" s="225"/>
-      <c r="K53" s="225"/>
-      <c r="L53" s="241" t="s">
+      <c r="H53" s="226"/>
+      <c r="I53" s="226"/>
+      <c r="J53" s="226"/>
+      <c r="K53" s="226"/>
+      <c r="L53" s="242" t="s">
         <v>119</v>
       </c>
-      <c r="M53" s="241"/>
-      <c r="N53" s="241"/>
+      <c r="M53" s="242"/>
+      <c r="N53" s="242"/>
       <c r="P53" s="21"/>
       <c r="Q53" s="23" t="s">
         <v>120</v>
@@ -5357,11 +5366,11 @@
       <c r="T53" s="23"/>
       <c r="U53" s="23"/>
       <c r="V53" s="23"/>
-      <c r="Z53" s="242" t="s">
+      <c r="Z53" s="243" t="s">
         <v>121</v>
       </c>
-      <c r="AA53" s="242"/>
-      <c r="AB53" s="242"/>
+      <c r="AA53" s="243"/>
+      <c r="AB53" s="243"/>
     </row>
   </sheetData>
   <mergeCells count="433">
@@ -5824,10 +5833,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5">
-      <c r="A1" s="258" t="s">
+      <c r="A1" s="259" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="258"/>
+      <c r="B1" s="259"/>
     </row>
     <row r="2" spans="1:2" ht="50.1" customHeight="1">
       <c r="A2" s="10" t="s">
@@ -5861,10 +5870,10 @@
     </row>
     <row r="6" spans="1:2" ht="20.25" customHeight="1"/>
     <row r="7" spans="1:2" ht="16.5">
-      <c r="A7" s="258" t="s">
+      <c r="A7" s="259" t="s">
         <v>122</v>
       </c>
-      <c r="B7" s="258"/>
+      <c r="B7" s="259"/>
     </row>
     <row r="8" spans="1:2" ht="50.1" customHeight="1">
       <c r="A8" s="10" t="s">
@@ -5900,10 +5909,10 @@
     </row>
     <row r="12" spans="1:2" ht="20.25" customHeight="1"/>
     <row r="13" spans="1:2" ht="16.5">
-      <c r="A13" s="258" t="s">
+      <c r="A13" s="259" t="s">
         <v>122</v>
       </c>
-      <c r="B13" s="258"/>
+      <c r="B13" s="259"/>
     </row>
     <row r="14" spans="1:2" ht="50.1" customHeight="1">
       <c r="A14" s="10" t="s">
@@ -5969,10 +5978,10 @@
       <c r="A1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="258" t="s">
+      <c r="B1" s="259" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="258"/>
+      <c r="C1" s="259"/>
       <c r="D1" s="1" t="s">
         <v>126</v>
       </c>
@@ -6466,7 +6475,7 @@
       <c r="C30" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="D30" s="258" t="s">
+      <c r="D30" s="259" t="s">
         <v>167</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -6483,7 +6492,7 @@
       <c r="C31" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="D31" s="258"/>
+      <c r="D31" s="259"/>
       <c r="E31" s="1" t="s">
         <v>138</v>
       </c>
@@ -6498,7 +6507,7 @@
       <c r="C32" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="D32" s="258"/>
+      <c r="D32" s="259"/>
       <c r="E32" s="1" t="s">
         <v>138</v>
       </c>
@@ -6513,7 +6522,7 @@
       <c r="C33" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="D33" s="258" t="s">
+      <c r="D33" s="259" t="s">
         <v>169</v>
       </c>
       <c r="E33" s="1" t="s">
@@ -6530,7 +6539,7 @@
       <c r="C34" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="D34" s="258"/>
+      <c r="D34" s="259"/>
       <c r="E34" s="1" t="s">
         <v>138</v>
       </c>
@@ -6545,7 +6554,7 @@
       <c r="C35" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="D35" s="258" t="s">
+      <c r="D35" s="259" t="s">
         <v>171</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -6562,7 +6571,7 @@
       <c r="C36" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="D36" s="258"/>
+      <c r="D36" s="259"/>
       <c r="E36" s="1" t="s">
         <v>138</v>
       </c>
@@ -6577,7 +6586,7 @@
       <c r="C37" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="D37" s="258"/>
+      <c r="D37" s="259"/>
       <c r="E37" s="1" t="s">
         <v>138</v>
       </c>

</xml_diff>